<commit_message>
featura: Natan Criação classes Usuario e Oferta
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\uau\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6960409-ACCF-4D08-8B5D-A313A966A072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C97DFCC-7E1C-4AD3-A556-12A476C91A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
   <si>
     <t>Id do produto</t>
   </si>
@@ -282,9 +282,6 @@
   </si>
   <si>
     <t>00001</t>
-  </si>
-  <si>
-    <t>Coca-Cola</t>
   </si>
   <si>
     <t>Lata - 250ml</t>
@@ -2677,16 +2674,16 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2711,7 +2708,7 @@
         <v>76</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C2" s="41">
         <v>10</v>
@@ -2720,15 +2717,15 @@
         <v>2.9</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="44" t="s">
         <v>79</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>80</v>
       </c>
       <c r="C3" s="45">
         <v>5</v>
@@ -2737,15 +2734,15 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>82</v>
       </c>
       <c r="C4" s="45">
         <v>15</v>
@@ -2754,15 +2751,15 @@
         <v>7</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="44" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>85</v>
       </c>
       <c r="C5" s="45">
         <v>5</v>
@@ -2771,15 +2768,15 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="44" t="s">
         <v>86</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>87</v>
       </c>
       <c r="C6" s="45">
         <v>3</v>
@@ -2788,15 +2785,15 @@
         <v>2</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>89</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>90</v>
       </c>
       <c r="C7" s="45">
         <v>20</v>
@@ -2805,7 +2802,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2824,10 +2821,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2863,10 +2860,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2944,13 +2941,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3027,9 +3024,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3083,15 +3080,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="4" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="28.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="30.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="29.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="18.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="27.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="5" width="30.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="4" width="27.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="27.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3544,9 +3541,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3639,15 +3636,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3750,11 +3747,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3867,14 +3864,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3919,10 +3916,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3969,14 +3966,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4021,9 +4018,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: atualizando arquivo excel
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\uau\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C97DFCC-7E1C-4AD3-A556-12A476C91A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF6C884-8631-4AED-880A-1ACFD1CA882E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Produto" sheetId="15" r:id="rId1"/>
+    <sheet name="Produto" sheetId="1" r:id="rId1"/>
     <sheet name="Estoque" sheetId="2" r:id="rId2"/>
     <sheet name="Vendas" sheetId="3" r:id="rId3"/>
     <sheet name="Fornecedores" sheetId="4" r:id="rId4"/>
@@ -51,9 +51,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
-  <si>
-    <t>Id do produto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+  <si>
+    <t>Id do Produto</t>
+  </si>
+  <si>
+    <t>Nome do Produto</t>
   </si>
   <si>
     <t xml:space="preserve">Quantidade do Produto </t>
@@ -65,6 +68,36 @@
     <t xml:space="preserve">Descrição de produto </t>
   </si>
   <si>
+    <t>Cola-Cola</t>
+  </si>
+  <si>
+    <t>Lata - 250ml</t>
+  </si>
+  <si>
+    <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Fanta Laranja</t>
+  </si>
+  <si>
+    <t>PET - 2L</t>
+  </si>
+  <si>
+    <t>Coca-Cola Zero</t>
+  </si>
+  <si>
+    <t>Água Mineral</t>
+  </si>
+  <si>
+    <t>PET - 350ml</t>
+  </si>
+  <si>
+    <t>Heineken</t>
+  </si>
+  <si>
+    <t>Lata - 350ml</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nome do produto </t>
   </si>
   <si>
@@ -128,13 +161,13 @@
     <t>Frigorificos</t>
   </si>
   <si>
-    <t>Vendas</t>
-  </si>
-  <si>
-    <t>Comissões</t>
-  </si>
-  <si>
-    <t>Compras</t>
+    <t>id Meta</t>
+  </si>
+  <si>
+    <t>Valor Da Meta</t>
+  </si>
+  <si>
+    <t>Bonificação</t>
   </si>
   <si>
     <t>idVendedor</t>
@@ -143,6 +176,15 @@
     <t>idCaixa</t>
   </si>
   <si>
+    <t>Data Inicio</t>
+  </si>
+  <si>
+    <t>Data Final</t>
+  </si>
+  <si>
+    <t>Valor de Vendas</t>
+  </si>
+  <si>
     <t>id Oferta</t>
   </si>
   <si>
@@ -170,7 +212,7 @@
     <t xml:space="preserve">Nome </t>
   </si>
   <si>
-    <t xml:space="preserve">CPF / RG </t>
+    <t xml:space="preserve">CPF </t>
   </si>
   <si>
     <t xml:space="preserve">CEP </t>
@@ -245,7 +287,13 @@
     <t>salario</t>
   </si>
   <si>
-    <t>cargoSetor</t>
+    <t>Cargo Setor</t>
+  </si>
+  <si>
+    <t>Situação</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
   <si>
     <t>ID Usuario</t>
@@ -275,68 +323,29 @@
     <t>Horario Logoff</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>Nome do Produto</t>
-  </si>
-  <si>
     <t>00001</t>
   </si>
   <si>
-    <t>Lata - 250ml</t>
-  </si>
-  <si>
     <t>00002</t>
   </si>
   <si>
-    <t>Pepsi</t>
-  </si>
-  <si>
     <t>00003</t>
   </si>
   <si>
-    <t>Fanta Laranja</t>
-  </si>
-  <si>
-    <t>PET - 2L</t>
-  </si>
-  <si>
     <t>00004</t>
   </si>
   <si>
-    <t>Coca-Cola Zero</t>
-  </si>
-  <si>
     <t>00005</t>
   </si>
   <si>
-    <t>Água Mineral</t>
-  </si>
-  <si>
-    <t>PET - 350ml</t>
-  </si>
-  <si>
     <t>00006</t>
-  </si>
-  <si>
-    <t>Heineken</t>
-  </si>
-  <si>
-    <t>Lata - 350ml</t>
-  </si>
-  <si>
-    <t>Cola</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,15 +377,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,8 +409,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBE2D5"/>
+        <bgColor rgb="FFFBE2D5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -544,11 +564,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF1A983"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF1A983"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF1A983"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -614,27 +664,28 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+  <dxfs count="97">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -643,11 +694,12 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -658,11 +710,12 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
@@ -671,6 +724,8 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -925,6 +980,54 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
         <right/>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -1371,6 +1474,78 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
         <right/>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -2032,84 +2207,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
-      <border>
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border>
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -2173,28 +2282,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" tableBorderDxfId="94" totalsRowBorderDxfId="93">
   <autoFilter ref="A1:E7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do produto" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:E7" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="A1:E7" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="cargoSetor" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+  <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2217,8 +2328,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C4" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
@@ -2229,50 +2340,53 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9AAC040D-6972-42A3-8D20-2F0B8DFC00F9}" name="Tabela8" displayName="Tabela8" ref="A1:I100" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9AAC040D-6972-42A3-8D20-2F0B8DFC00F9}" name="Tabela8" displayName="Tabela8" ref="A1:I100" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85">
   <autoFilter ref="A1:I100" xr:uid="{9AAC040D-6972-42A3-8D20-2F0B8DFC00F9}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2FC4FD4D-D942-4D2B-9C9B-EDE6042DABFD}" name="Nome do produto " dataDxfId="79"/>
-    <tableColumn id="2" xr3:uid="{DCD298EB-EAE8-4E25-B35D-673BABAD6CBE}" name="Data de validade " dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{357D547E-A836-42BB-BEC0-586734D3064B}" name="Data de entrada do produto " dataDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{76E1D021-317F-45F3-B626-4DA7E2401097}" name="Quantidade de Entada do produto" dataDxfId="76"/>
-    <tableColumn id="5" xr3:uid="{C01DCEB5-2EAF-4234-A5CC-44A5F9CD43E5}" name="Valor de entrada do produto " dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{AF7978DF-FF29-4ECD-A699-9AD28B29DBF4}" name="Codigo de barras " dataDxfId="74"/>
-    <tableColumn id="7" xr3:uid="{0C12CD58-4C4C-4C4E-8AE6-489C00D8A9D3}" name="Codigo interno do produto " dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{5C815496-DEC9-41C5-AC21-851858E322E2}" name="Quantidade de perca de estoque " dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{E80ECE3E-A9CA-4A11-BAC7-ED7274E5A723}" name="Valor de perca de estoque " dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{2FC4FD4D-D942-4D2B-9C9B-EDE6042DABFD}" name="Nome do produto " dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{DCD298EB-EAE8-4E25-B35D-673BABAD6CBE}" name="Data de validade " dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{357D547E-A836-42BB-BEC0-586734D3064B}" name="Data de entrada do produto " dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{76E1D021-317F-45F3-B626-4DA7E2401097}" name="Quantidade de Entada do produto" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{C01DCEB5-2EAF-4234-A5CC-44A5F9CD43E5}" name="Valor de entrada do produto " dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{AF7978DF-FF29-4ECD-A699-9AD28B29DBF4}" name="Codigo de barras " dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{0C12CD58-4C4C-4C4E-8AE6-489C00D8A9D3}" name="Codigo interno do produto " dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{5C815496-DEC9-41C5-AC21-851858E322E2}" name="Quantidade de perca de estoque " dataDxfId="77"/>
+    <tableColumn id="9" xr3:uid="{E80ECE3E-A9CA-4A11-BAC7-ED7274E5A723}" name="Valor de perca de estoque " dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:I6" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67" totalsRowBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:I6" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="A1:I6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Varejistas" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="idVarejistas" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{CC43FF0E-343A-4BE8-B3ED-BDD2BE086AF5}" name="Atacadistas" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{25A239E3-CCB4-435B-81B9-F65438B2AAA8}" name="idAtacadistas" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{D5A30311-B824-4B2C-915D-5B791775130C}" name="Industrias" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{E21EC659-BC19-4AA6-9315-BBB4A49D7680}" name="idIndustrias" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Alimenticios" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Laticinios" dataDxfId="58"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Frigorificos" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Varejistas" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="idVarejistas" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{CC43FF0E-343A-4BE8-B3ED-BDD2BE086AF5}" name="Atacadistas" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{25A239E3-CCB4-435B-81B9-F65438B2AAA8}" name="idAtacadistas" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{D5A30311-B824-4B2C-915D-5B791775130C}" name="Industrias" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{E21EC659-BC19-4AA6-9315-BBB4A49D7680}" name="idIndustrias" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Alimenticios" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Laticinios" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Frigorificos" dataDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:E12" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
-  <autoFilter ref="A1:E12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="Vendas" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Comissões" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Compras" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+  <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2296,22 +2410,22 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF / RG " dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:H2" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{54DD2ABE-9EAE-463E-96A5-779CE8C6809A}" name="id Produto"/>
@@ -2328,13 +2442,13 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2670,143 +2784,143 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F58C0B-57E8-4276-8810-DFFB47197267}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="41">
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="46">
         <v>10</v>
       </c>
       <c r="D2" s="42">
         <v>2.9</v>
       </c>
-      <c r="E2" s="43" t="s">
-        <v>77</v>
+      <c r="E2" s="38" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="45">
+      <c r="A3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="47">
         <v>5</v>
       </c>
-      <c r="D3" s="46">
+      <c r="D3" s="43">
         <v>2.5</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>77</v>
+      <c r="E3" s="39" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="45">
+      <c r="A4" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="48">
         <v>15</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="44">
         <v>7</v>
       </c>
-      <c r="E4" s="47" t="s">
-        <v>82</v>
+      <c r="E4" s="40" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="45">
+      <c r="A5" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="47">
         <v>5</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="43">
         <v>2.5</v>
       </c>
-      <c r="E5" s="47" t="s">
-        <v>77</v>
+      <c r="E5" s="39" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="45">
+      <c r="A6" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="48">
         <v>3</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="44">
         <v>2</v>
       </c>
-      <c r="E6" s="47" t="s">
-        <v>87</v>
+      <c r="E6" s="40" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="45">
+      <c r="A7" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="49">
         <v>20</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="45">
         <v>4</v>
       </c>
-      <c r="E7" s="47" t="s">
-        <v>90</v>
+      <c r="E7" s="41" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2821,27 +2935,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2854,76 +2968,124 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A4EF80-7496-4B05-86B1-54C8E4F6E45F}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="24"/>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="26"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="26"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
       <c r="E7" s="29"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2941,36 +3103,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3016,51 +3178,32 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="36">
-        <v>0.52106481481481481</v>
-      </c>
-      <c r="C2" s="37">
-        <v>0.54236111111111107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="E4" s="38"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3075,49 +3218,49 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="27.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3541,20 +3684,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3636,44 +3779,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3741,112 +3884,159 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490B7451-1A7F-4FCB-BE82-E7B49B8D5224}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="32"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="36"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="26"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="26"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
       <c r="E7" s="26"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
       <c r="E8" s="26"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3864,40 +4054,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3912,34 +4102,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13400A9C-35AF-4D1A-A093-BF6B7D89743A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3966,40 +4160,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -4018,23 +4212,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="E1" s="3"/>
     </row>

</xml_diff>

<commit_message>
fix: Tabelas Estoque e Venda Excel
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -1,35 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\uau\mercadoFacil-piSenac-\src\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF6C884-8631-4AED-880A-1ACFD1CA882E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68613A82-EDDC-46F3-9DD0-44BDDEE3D27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
-    <sheet name="Estoque" sheetId="2" r:id="rId2"/>
-    <sheet name="Vendas" sheetId="3" r:id="rId3"/>
-    <sheet name="Fornecedores" sheetId="4" r:id="rId4"/>
-    <sheet name="Metas" sheetId="5" r:id="rId5"/>
-    <sheet name="Ofertas" sheetId="6" r:id="rId6"/>
-    <sheet name="Cliente" sheetId="7" r:id="rId7"/>
-    <sheet name="Compra" sheetId="8" r:id="rId8"/>
-    <sheet name="Empresa" sheetId="9" r:id="rId9"/>
-    <sheet name="Ponto Funcionarios" sheetId="10" r:id="rId10"/>
-    <sheet name="Funcionarios" sheetId="11" r:id="rId11"/>
-    <sheet name="Usuarios" sheetId="12" r:id="rId12"/>
-    <sheet name="Controle de Acesso" sheetId="14" r:id="rId13"/>
+    <sheet name="Estoque" sheetId="17" r:id="rId2"/>
+    <sheet name="Vendas" sheetId="15" r:id="rId3"/>
+    <sheet name="Venda_Produto" sheetId="16" r:id="rId4"/>
+    <sheet name="Fornecedores" sheetId="4" r:id="rId5"/>
+    <sheet name="Metas" sheetId="5" r:id="rId6"/>
+    <sheet name="Ofertas" sheetId="6" r:id="rId7"/>
+    <sheet name="Cliente" sheetId="7" r:id="rId8"/>
+    <sheet name="Compra" sheetId="8" r:id="rId9"/>
+    <sheet name="Empresa" sheetId="9" r:id="rId10"/>
+    <sheet name="Ponto Funcionarios" sheetId="10" r:id="rId11"/>
+    <sheet name="Funcionarios" sheetId="11" r:id="rId12"/>
+    <sheet name="Usuarios" sheetId="12" r:id="rId13"/>
+    <sheet name="Controle de Acesso" sheetId="14" r:id="rId14"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Vendas!$A$1:$C$1</definedName>
-  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -98,42 +96,6 @@
     <t>Lata - 350ml</t>
   </si>
   <si>
-    <t xml:space="preserve">Nome do produto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data de validade </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data de entrada do produto </t>
-  </si>
-  <si>
-    <t>Quantidade de Entada do produto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor de entrada do produto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codigo de barras </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codigo interno do produto </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quantidade de perca de estoque </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor de perca de estoque </t>
-  </si>
-  <si>
-    <t>Fluxo de Caixa</t>
-  </si>
-  <si>
-    <t>Emissão de Nota Fiscal</t>
-  </si>
-  <si>
-    <t>Promoção e Sorteios</t>
-  </si>
-  <si>
     <t>Varejistas</t>
   </si>
   <si>
@@ -185,27 +147,9 @@
     <t>Valor de Vendas</t>
   </si>
   <si>
-    <t>id Oferta</t>
-  </si>
-  <si>
-    <t>Data Criação</t>
-  </si>
-  <si>
     <t>Data Fim</t>
   </si>
   <si>
-    <t>Preço Antigo</t>
-  </si>
-  <si>
-    <t>Valor Promocional</t>
-  </si>
-  <si>
-    <t>Qtde Mínima</t>
-  </si>
-  <si>
-    <t>Percentual Desconto</t>
-  </si>
-  <si>
     <t>id Produto</t>
   </si>
   <si>
@@ -339,13 +283,76 @@
   </si>
   <si>
     <t>00006</t>
+  </si>
+  <si>
+    <t>Id Produto</t>
+  </si>
+  <si>
+    <t>Id Venda</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Parcelas</t>
+  </si>
+  <si>
+    <t>Observações</t>
+  </si>
+  <si>
+    <t>Id Vendedor</t>
+  </si>
+  <si>
+    <t>Forma Pagamento</t>
+  </si>
+  <si>
+    <t>Id Cliente</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Venda Id</t>
+  </si>
+  <si>
+    <t>Produto Id</t>
+  </si>
+  <si>
+    <t>Id Item Venda</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>Valor Item</t>
+  </si>
+  <si>
+    <t>Valor Venda</t>
+  </si>
+  <si>
+    <t>Id Lote</t>
+  </si>
+  <si>
+    <t>Data Validade</t>
+  </si>
+  <si>
+    <t>Custo</t>
+  </si>
+  <si>
+    <t>Data Entrada</t>
+  </si>
+  <si>
+    <t>Id Oferta</t>
+  </si>
+  <si>
+    <t>Desconto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,21 +364,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,7 +382,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,12 +392,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -609,21 +595,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -646,7 +620,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -662,28 +635,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="97">
+  <dxfs count="85">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1998,214 +1970,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -2282,20 +2046,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="84" headerRowBorderDxfId="83" tableBorderDxfId="82" totalsRowBorderDxfId="81">
   <autoFilter ref="A1:E7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}" name="Tabela6" displayName="Tabela6" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D05168A4-7494-42E3-80CA-A5EF91D04256}" name="data"/>
+    <tableColumn id="2" xr3:uid="{9125E824-2504-4B0E-957D-030859DB5451}" name="id Funcionario"/>
+    <tableColumn id="3" xr3:uid="{A0BF47A2-E842-4FA4-A386-D0024C55EB45}" name="Horario Saída"/>
+    <tableColumn id="4" xr3:uid="{FB70219B-2083-4B01-9D13-7727ECC20C12}" name="Horario Entrada"/>
+    <tableColumn id="5" xr3:uid="{FEE7D022-5791-4930-BF05-5D2D5A1660B7}" name="Tempo Atraso"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
@@ -2311,7 +2102,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:G2" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="7">
@@ -2327,7 +2118,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
@@ -2340,24 +2131,53 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9AAC040D-6972-42A3-8D20-2F0B8DFC00F9}" name="Tabela8" displayName="Tabela8" ref="A1:I100" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85">
-  <autoFilter ref="A1:I100" xr:uid="{9AAC040D-6972-42A3-8D20-2F0B8DFC00F9}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{2FC4FD4D-D942-4D2B-9C9B-EDE6042DABFD}" name="Nome do produto " dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{DCD298EB-EAE8-4E25-B35D-673BABAD6CBE}" name="Data de validade " dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{357D547E-A836-42BB-BEC0-586734D3064B}" name="Data de entrada do produto " dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{76E1D021-317F-45F3-B626-4DA7E2401097}" name="Quantidade de Entada do produto" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{C01DCEB5-2EAF-4234-A5CC-44A5F9CD43E5}" name="Valor de entrada do produto " dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{AF7978DF-FF29-4ECD-A699-9AD28B29DBF4}" name="Codigo de barras " dataDxfId="79"/>
-    <tableColumn id="7" xr3:uid="{0C12CD58-4C4C-4C4E-8AE6-489C00D8A9D3}" name="Codigo interno do produto " dataDxfId="78"/>
-    <tableColumn id="8" xr3:uid="{5C815496-DEC9-41C5-AC21-851858E322E2}" name="Quantidade de perca de estoque " dataDxfId="77"/>
-    <tableColumn id="9" xr3:uid="{E80ECE3E-A9CA-4A11-BAC7-ED7274E5A723}" name="Valor de perca de estoque " dataDxfId="76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}" name="Tabela13" displayName="Tabela13" ref="A1:I2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{7DA33DF1-70D3-4985-AD72-C7C4CD7A129D}" name="Id Venda"/>
+    <tableColumn id="9" xr3:uid="{26C688A1-DD2C-49A5-9C45-F5670E955BE3}" name="Data"/>
+    <tableColumn id="2" xr3:uid="{B3F389AE-D3A8-4AE7-9533-7F15BEA25591}" name="Hora"/>
+    <tableColumn id="3" xr3:uid="{F3B8F060-BA34-4591-8528-611FE4C95156}" name="Valor Venda"/>
+    <tableColumn id="4" xr3:uid="{F23EAAFB-7C1A-4B89-8679-77D9B852568E}" name="Forma Pagamento"/>
+    <tableColumn id="5" xr3:uid="{BE3D88F9-0263-4A0C-B707-F4991ADEB5D1}" name="Parcelas"/>
+    <tableColumn id="6" xr3:uid="{94D5006F-82D0-4B41-93D5-12F2E5575674}" name="Observações"/>
+    <tableColumn id="7" xr3:uid="{15730F61-DC8B-47AA-A898-94B46456C062}" name="Id Vendedor"/>
+    <tableColumn id="8" xr3:uid="{89AAD5BB-19E7-43F2-9F59-EB4FD699DC56}" name="Id Cliente"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}" name="Tabela14" displayName="Tabela14" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6A285388-05C3-4250-931A-479D682F6087}" name="Id Item Venda"/>
+    <tableColumn id="2" xr3:uid="{13A3B266-03F3-4868-A4D9-FC39B364494E}" name="Venda Id"/>
+    <tableColumn id="3" xr3:uid="{C6DD3B99-EBEF-4F4B-96E3-96DC3228A5FD}" name="Produto Id"/>
+    <tableColumn id="4" xr3:uid="{685D0BE6-1F42-4049-BE66-811D246CDE37}" name="Quantidade"/>
+    <tableColumn id="5" xr3:uid="{20C600D2-E04C-46CF-B028-B45422F121D1}" name="Valor Item"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:I6" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="A1:I6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="9">
@@ -2375,7 +2195,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
@@ -2392,24 +2212,21 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="id Oferta"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Data Criação"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Data Fim"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Preço Antigo"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Valor Promocional"/>
-    <tableColumn id="6" xr3:uid="{4BFE1514-66DD-4060-8211-B7317342F515}" name="Qtde Mínima"/>
-    <tableColumn id="7" xr3:uid="{534E9D70-7974-45F4-BBA8-C87F5AA24600}" name="Percentual Desconto"/>
-    <tableColumn id="8" xr3:uid="{CD7E370C-6838-423A-A0E7-135FBD230535}" name="id Produto"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
@@ -2424,7 +2241,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A1:H2" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}"/>
   <tableColumns count="8">
@@ -2438,33 +2255,6 @@
     <tableColumn id="8" xr3:uid="{C68A7FDB-58C6-405F-ACC9-2F261CB1A345}" name="Previsão Entrega"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
-  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="30"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}" name="Tabela6" displayName="Tabela6" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D05168A4-7494-42E3-80CA-A5EF91D04256}" name="data"/>
-    <tableColumn id="2" xr3:uid="{9125E824-2504-4B0E-957D-030859DB5451}" name="id Funcionario"/>
-    <tableColumn id="3" xr3:uid="{A0BF47A2-E842-4FA4-A386-D0024C55EB45}" name="Horario Saída"/>
-    <tableColumn id="4" xr3:uid="{FB70219B-2083-4B01-9D13-7727ECC20C12}" name="Horario Entrada"/>
-    <tableColumn id="5" xr3:uid="{FEE7D022-5791-4930-BF05-5D2D5A1660B7}" name="Tempo Atraso"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2787,7 +2577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2801,121 +2591,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="38">
         <v>10</v>
       </c>
-      <c r="D2" s="42">
+      <c r="D2" s="34">
         <v>2.9</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="30" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="39" t="s">
+      <c r="A3" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="39">
         <v>5</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="35">
         <v>2.5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="48">
+      <c r="C4" s="40">
         <v>15</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="36">
         <v>7</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="39" t="s">
+      <c r="A5" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="39">
         <v>5</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="35">
         <v>2.5</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="31" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="40">
         <v>3</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="36">
         <v>2</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="41">
         <v>20</v>
       </c>
-      <c r="D7" s="45">
+      <c r="D7" s="37">
         <v>4</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2928,6 +2718,48 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2C0B43-F228-4CBF-98A3-FF8522669C40}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E75FFB4-713F-4EF0-9034-135108041187}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -2943,19 +2775,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2966,7 +2798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A4EF80-7496-4B05-86B1-54C8E4F6E45F}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -2984,108 +2816,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>80</v>
+      <c r="A1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3095,7 +2927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41E1062-872E-487D-8046-A7F258A4D356}">
   <dimension ref="A1:G10"/>
   <sheetViews>
@@ -3113,60 +2945,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>86</v>
+      <c r="A1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="21"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="22"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="22"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="22"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="22"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="22"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="22"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="22"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="22"/>
+      <c r="G10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3176,7 +3008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3190,20 +3022,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>89</v>
+      <c r="A1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3214,460 +3046,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF0487D-EF1B-4DB2-B3CD-F0E7AF28F1C9}">
-  <dimension ref="A1:I100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FCEB4-E501-4D56-BC91-46B2FB941374}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="10"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="10"/>
-      <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="10"/>
-      <c r="I50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="I51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="I52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="10"/>
-      <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="I54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10"/>
-      <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="10"/>
-      <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="10"/>
-      <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="10"/>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="10"/>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="10"/>
-      <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="10"/>
-      <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="10"/>
-      <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
-      <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="10"/>
-      <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="10"/>
-      <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="10"/>
-      <c r="I70" s="5"/>
-    </row>
-    <row r="71" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10"/>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
-      <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
-      <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
-      <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="10"/>
-      <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="10"/>
-      <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
-      <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="10"/>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="10"/>
-      <c r="I84" s="5"/>
-    </row>
-    <row r="85" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="10"/>
-      <c r="I85" s="5"/>
-    </row>
-    <row r="86" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="10"/>
-      <c r="I86" s="5"/>
-    </row>
-    <row r="87" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
-      <c r="I87" s="5"/>
-    </row>
-    <row r="88" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="10"/>
-      <c r="I88" s="5"/>
-    </row>
-    <row r="89" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="10"/>
-      <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="10"/>
-      <c r="I90" s="5"/>
-    </row>
-    <row r="91" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="10"/>
-      <c r="I91" s="5"/>
-    </row>
-    <row r="92" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="10"/>
-      <c r="I92" s="5"/>
-    </row>
-    <row r="93" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="10"/>
-      <c r="I93" s="5"/>
-    </row>
-    <row r="94" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="10"/>
-      <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
-      <c r="I95" s="5"/>
-    </row>
-    <row r="96" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="10"/>
-      <c r="I96" s="5"/>
-    </row>
-    <row r="97" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
-      <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="10"/>
-      <c r="I98" s="5"/>
-    </row>
-    <row r="99" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="10"/>
-      <c r="I99" s="5"/>
-    </row>
-    <row r="100" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="14"/>
-      <c r="I100" s="14"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3675,107 +3091,110 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E854437E-ED2A-41DC-912E-2B17F37C4A64}">
-  <dimension ref="A1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874DB2D-2BBA-4881-96E3-9EC756E4450A}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="25"/>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{E854437E-ED2A-41DC-912E-2B17F37C4A64}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124AE1B6-FA2F-480E-B92D-4A36EA8A4444}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B46210-C88C-4D3D-AA28-7F5B038AF542}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3791,88 +3210,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>35</v>
+      <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="26"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="26"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="29"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3882,7 +3301,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490B7451-1A7F-4FCB-BE82-E7B49B8D5224}">
   <dimension ref="A1:H12"/>
   <sheetViews>
@@ -3903,192 +3322,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>43</v>
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="36"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E452B3BA-6480-4C31-A0A0-FCD7F2BD6829}">
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4099,6 +3466,50 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E452B3BA-6480-4C31-A0A0-FCD7F2BD6829}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13400A9C-35AF-4D1A-A093-BF6B7D89743A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4117,32 +3528,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>57</v>
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4152,7 +3563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA874376-F7A1-44D3-877B-097ED91B3546}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -4172,71 +3583,29 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2C0B43-F228-4CBF-98A3-FF8522669C40}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: campos de tabela fornecedores
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A563A4B-5BDD-413E-92C1-EB846FA30A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB05E62-CF19-44A3-8E56-D7915D412209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -96,33 +96,6 @@
     <t>Lata - 350ml</t>
   </si>
   <si>
-    <t>Varejistas</t>
-  </si>
-  <si>
-    <t>idVarejistas</t>
-  </si>
-  <si>
-    <t>Atacadistas</t>
-  </si>
-  <si>
-    <t>idAtacadistas</t>
-  </si>
-  <si>
-    <t>Industrias</t>
-  </si>
-  <si>
-    <t>idIndustrias</t>
-  </si>
-  <si>
-    <t>Alimenticios</t>
-  </si>
-  <si>
-    <t>Laticinios</t>
-  </si>
-  <si>
-    <t>Frigorificos</t>
-  </si>
-  <si>
     <t>id Meta</t>
   </si>
   <si>
@@ -346,6 +319,24 @@
   </si>
   <si>
     <t>Desconto</t>
+  </si>
+  <si>
+    <t>Id Fornecedor</t>
+  </si>
+  <si>
+    <t>Tipo Comércio</t>
+  </si>
+  <si>
+    <t>Endereço</t>
+  </si>
+  <si>
+    <t>Responsável</t>
+  </si>
+  <si>
+    <t>Nome Fornecedor</t>
+  </si>
+  <si>
+    <t>Documento</t>
   </si>
 </sst>
 </file>
@@ -655,7 +646,53 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="83">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1792,102 +1829,6 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
@@ -2046,27 +1987,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="84" headerRowBorderDxfId="83" tableBorderDxfId="82" totalsRowBorderDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A1:E7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="75"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="37" headerRowBorderDxfId="36" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2087,44 +2028,44 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="A1:G2" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2178,35 +2119,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:I6" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
-  <autoFilter ref="A1:I6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Varejistas" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="idVarejistas" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{CC43FF0E-343A-4BE8-B3ED-BDD2BE086AF5}" name="Atacadistas" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{25A239E3-CCB4-435B-81B9-F65438B2AAA8}" name="idAtacadistas" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{D5A30311-B824-4B2C-915D-5B791775130C}" name="Industrias" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{E21EC659-BC19-4AA6-9315-BBB4A49D7680}" name="idIndustrias" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Alimenticios" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Laticinios" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Frigorificos" dataDxfId="62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+  <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="65"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2227,22 +2166,22 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="40">
   <autoFilter ref="A1:H2" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{54DD2ABE-9EAE-463E-96A5-779CE8C6809A}" name="id Produto"/>
@@ -2609,7 +2548,7 @@
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B2" s="30" t="s">
         <v>5</v>
@@ -2626,7 +2565,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>7</v>
@@ -2643,7 +2582,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>8</v>
@@ -2660,7 +2599,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B5" s="31" t="s">
         <v>10</v>
@@ -2677,7 +2616,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>11</v>
@@ -2694,7 +2633,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>13</v>
@@ -2732,16 +2671,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E1" s="3"/>
     </row>
@@ -2775,19 +2714,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2817,25 +2756,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2946,25 +2885,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3012,7 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3023,13 +2962,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3064,22 +3003,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3111,31 +3050,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3150,7 +3089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124AE1B6-FA2F-480E-B92D-4A36EA8A4444}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3165,19 +3104,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3190,108 +3129,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B46210-C88C-4D3D-AA28-7F5B038AF542}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>20</v>
+        <v>92</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="19"/>
+      <c r="G2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3323,28 +3244,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,19 +3407,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3513,7 +3434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13400A9C-35AF-4D1A-A093-BF6B7D89743A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3529,22 +3450,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3583,28 +3504,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: classe gerenciadora de compras com adição de campo id compra em planilha
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB05E62-CF19-44A3-8E56-D7915D412209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D88EB0-8BD4-4F31-B425-B9C4F09BD6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Metas" sheetId="5" r:id="rId6"/>
     <sheet name="Ofertas" sheetId="6" r:id="rId7"/>
     <sheet name="Cliente" sheetId="7" r:id="rId8"/>
-    <sheet name="Compra" sheetId="8" r:id="rId9"/>
+    <sheet name="Compra" sheetId="18" r:id="rId9"/>
     <sheet name="Empresa" sheetId="9" r:id="rId10"/>
     <sheet name="Ponto Funcionarios" sheetId="10" r:id="rId11"/>
     <sheet name="Funcionarios" sheetId="11" r:id="rId12"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Data Fim</t>
   </si>
   <si>
-    <t>id Produto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nome </t>
   </si>
   <si>
@@ -337,6 +334,15 @@
   </si>
   <si>
     <t>Documento</t>
+  </si>
+  <si>
+    <t>Lata 350ml</t>
+  </si>
+  <si>
+    <t>id Compra</t>
+  </si>
+  <si>
+    <t>id Produto2</t>
   </si>
 </sst>
 </file>
@@ -575,11 +581,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,56 +645,44 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+  <dxfs count="92">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1329,9 +1320,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1738,7 +1726,9 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -1760,9 +1750,7 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
+        <right/>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -1808,6 +1796,52 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
@@ -1987,27 +2021,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
   <autoFilter ref="A1:E7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2028,44 +2062,44 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A1:G2" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2119,33 +2153,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79" totalsRowBorderDxfId="78">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="63" dataDxfId="61" headerRowBorderDxfId="62" tableBorderDxfId="60" totalsRowBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67" totalsRowBorderDxfId="66">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="62"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="61"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="60"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2166,32 +2200,33 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="50" dataDxfId="48" headerRowBorderDxfId="49" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0" headerRowDxfId="40">
-  <autoFilter ref="A1:H2" xr:uid="{62D7D0C6-09C6-495D-97D7-E13D2FC6FE7E}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{54DD2ABE-9EAE-463E-96A5-779CE8C6809A}" name="id Produto"/>
-    <tableColumn id="2" xr3:uid="{5D57DB20-7DA1-4498-B707-73D6816CB589}" name="Data Solitação"/>
-    <tableColumn id="3" xr3:uid="{289765F1-0C9E-4A81-8396-27361C235D2D}" name="Valor Unitário"/>
-    <tableColumn id="4" xr3:uid="{BA296A65-2AF0-4DA0-9D2F-41339CB43C8F}" name="Unidade Medida"/>
-    <tableColumn id="5" xr3:uid="{DEB38209-E03B-4D4C-BF28-901374268048}" name="Valor Total"/>
-    <tableColumn id="6" xr3:uid="{09C20FE0-1237-48C8-B13B-149FC3C03296}" name="Qtde Total"/>
-    <tableColumn id="7" xr3:uid="{35923607-2E8D-4C1D-A92C-37476B1E162A}" name="id Fornecedor"/>
-    <tableColumn id="8" xr3:uid="{C68A7FDB-58C6-405F-ACC9-2F261CB1A345}" name="Previsão Entrega"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2517,7 +2552,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,121 +2565,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="37">
+        <v>10</v>
+      </c>
+      <c r="D2" s="33">
+        <v>2.9</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="38">
         <v>5</v>
       </c>
-      <c r="C2" s="38">
+      <c r="D3" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="39">
+        <v>15</v>
+      </c>
+      <c r="D4" s="35">
+        <v>7</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="34">
-        <v>2.9</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="C5" s="38">
+        <v>5</v>
+      </c>
+      <c r="D5" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="39">
-        <v>5</v>
-      </c>
-      <c r="D3" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="40">
-        <v>15</v>
-      </c>
-      <c r="D4" s="36">
-        <v>7</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="39">
-        <v>5</v>
-      </c>
-      <c r="D5" s="35">
-        <v>2.5</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="B6" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="39">
+        <v>3</v>
+      </c>
+      <c r="D6" s="35">
+        <v>2</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="40">
-        <v>3</v>
-      </c>
-      <c r="D6" s="36">
-        <v>2</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>20</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>4</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2670,25 +2705,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2714,19 +2749,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2755,108 +2790,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2884,60 +2919,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="15"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G3" s="16"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="16"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="16"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="16"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="16"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="16"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="16"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="16"/>
+      <c r="G10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2951,7 +2986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2961,20 +2998,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3003,22 +3040,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3050,31 +3087,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>71</v>
       </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3104,19 +3141,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>81</v>
-      </c>
-      <c r="E1" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3147,72 +3184,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="18"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="18"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="17"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="21"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3243,140 +3280,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="28"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3407,13 +3444,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -3449,32 +3486,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3485,51 +3522,85 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA874376-F7A1-44D3-877B-097ED91B3546}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F54BC8-357B-48B5-9891-582B5BE6F66B}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="42">
+        <v>45402</v>
+      </c>
+      <c r="D2" s="43">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="43">
+        <v>200</v>
+      </c>
+      <c r="G2" s="44">
+        <v>80</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="42">
+        <v>45408</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
fix: Classe, Gerenciador e Planilha Produto
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D88EB0-8BD4-4F31-B425-B9C4F09BD6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E10C1B-03AC-49F5-9F76-35A1716A8E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="107">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Nome do Produto</t>
   </si>
   <si>
-    <t xml:space="preserve">Quantidade do Produto </t>
-  </si>
-  <si>
     <t xml:space="preserve">Valor do Produto </t>
   </si>
   <si>
@@ -343,6 +340,36 @@
   </si>
   <si>
     <t>id Produto2</t>
+  </si>
+  <si>
+    <t>Código de Barra</t>
+  </si>
+  <si>
+    <t>00125091</t>
+  </si>
+  <si>
+    <t>00125092</t>
+  </si>
+  <si>
+    <t>00125093</t>
+  </si>
+  <si>
+    <t>00125094</t>
+  </si>
+  <si>
+    <t>00125095</t>
+  </si>
+  <si>
+    <t>00125096</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Refrigerante</t>
+  </si>
+  <si>
+    <t>Cerveja</t>
   </si>
 </sst>
 </file>
@@ -581,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -641,10 +668,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -653,36 +676,69 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
-    <dxf>
+  <dxfs count="93">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFF1A983"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1320,6 +1376,36 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1948,18 +2034,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color rgb="FF000000"/>
@@ -2021,27 +2095,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:E7" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="A1:E7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Quantidade do Produto " dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="83"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="92" headerRowBorderDxfId="91" tableBorderDxfId="90" totalsRowBorderDxfId="89">
+  <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" headerRowBorderDxfId="46" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2062,44 +2137,44 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G2" insertRow="1" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A1:G2" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2153,33 +2228,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="82" dataDxfId="80" headerRowBorderDxfId="81" tableBorderDxfId="79" totalsRowBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="87" dataDxfId="85" headerRowBorderDxfId="86" tableBorderDxfId="84" totalsRowBorderDxfId="83">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="71"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="80"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="79"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67" totalsRowBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="75" dataDxfId="73" headerRowBorderDxfId="74" tableBorderDxfId="72" totalsRowBorderDxfId="71">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="65"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="62"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="60"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="59"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2200,33 +2275,33 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="57" dataDxfId="55" headerRowBorderDxfId="56" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="52">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2549,10 +2624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,10 +2636,11 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2572,115 +2648,136 @@
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="37">
-        <v>10</v>
+      <c r="C2" s="29" t="s">
+        <v>98</v>
       </c>
       <c r="D2" s="33">
         <v>2.9</v>
       </c>
       <c r="E2" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="38">
-        <v>5</v>
+      <c r="C3" s="30" t="s">
+        <v>99</v>
       </c>
       <c r="D3" s="34">
         <v>2.5</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="39">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>100</v>
       </c>
       <c r="D4" s="35">
         <v>7</v>
       </c>
       <c r="E4" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="38">
-        <v>5</v>
+      <c r="C5" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="D5" s="34">
         <v>2.5</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="39">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>102</v>
       </c>
       <c r="D6" s="35">
         <v>2</v>
       </c>
       <c r="E6" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="40">
-        <v>20</v>
+      <c r="C7" s="32" t="s">
+        <v>103</v>
       </c>
       <c r="D7" s="36">
         <v>4</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>14</v>
+        <v>106</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2706,16 +2803,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="2"/>
     </row>
@@ -2749,19 +2846,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2791,25 +2888,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,25 +3017,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2999,13 +3096,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3040,22 +3137,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3087,31 +3184,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
         <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3141,19 +3238,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
-      </c>
-      <c r="E1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3185,25 +3282,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="D1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3281,28 +3378,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3444,19 +3541,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3487,22 +3584,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3525,7 +3622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F54BC8-357B-48B5-9891-582B5BE6F66B}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3543,59 +3640,59 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="42">
+      <c r="A2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="38">
         <v>45402</v>
       </c>
-      <c r="D2" s="43">
+      <c r="D2" s="39">
         <v>2.5</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="43">
+      <c r="E2" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="39">
         <v>200</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="40">
         <v>80</v>
       </c>
-      <c r="H2" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="42">
+      <c r="H2" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="38">
         <v>45408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: refatoração de classes gerenciadoras
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF7B043-954E-4B6C-AE59-C43496FE08D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5150E3A3-7630-4192-82B6-D15CD78B0796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Empresa" sheetId="9" r:id="rId10"/>
     <sheet name="Ponto Funcionarios" sheetId="10" r:id="rId11"/>
     <sheet name="Funcionarios" sheetId="11" r:id="rId12"/>
-    <sheet name="Usuarios" sheetId="12" r:id="rId13"/>
+    <sheet name="Usuarios" sheetId="19" r:id="rId13"/>
     <sheet name="Controle de Acesso" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Gerente</t>
+  </si>
+  <si>
+    <t>Id Funcionário</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -653,10 +656,42 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -665,7 +700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -692,9 +727,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -726,20 +758,43 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="94">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -760,127 +815,156 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -892,15 +976,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -908,6 +983,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -943,6 +1027,50 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
@@ -2134,28 +2262,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2176,44 +2304,45 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:G4" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:G4" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H4" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="5" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2267,33 +2396,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80" tableBorderDxfId="78" totalsRowBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="74"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="71"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="76"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="75"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="74"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="69" dataDxfId="67" headerRowBorderDxfId="68" tableBorderDxfId="66" totalsRowBorderDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="63"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="59"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="58"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2314,33 +2443,33 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2680,16 +2809,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2700,122 +2829,122 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>2.9</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <v>2.5</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="33">
         <v>7</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <v>2.5</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>2</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>4</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="30" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2913,7 +3042,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,85 +3078,85 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3038,26 +3167,27 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B41E1062-872E-487D-8046-A7F258A4D356}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540BAB3-B589-4DCB-98FE-D1E262F0FB3A}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -3072,67 +3202,76 @@
       <c r="E1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="46" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="H2" s="40" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="H3" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="44" t="s">
         <v>120</v>
       </c>
       <c r="D4" s="41" t="s">
@@ -3141,39 +3280,20 @@
       <c r="E4" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="47" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="14"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" s="14"/>
+      <c r="H4" s="41" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{E76427CC-732D-4292-85A7-D655B82EA141}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{64E20D12-016C-4B0E-9192-1FEF531FD847}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3403,49 +3523,49 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="16"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="16"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3502,114 +3622,114 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3767,31 +3887,31 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="36">
         <v>45402</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>2.5</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="38">
+      <c r="F2" s="37">
         <v>200</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="38">
         <v>80</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="37">
+      <c r="I2" s="36">
         <v>45408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: Gerenciador de Login
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5150E3A3-7630-4192-82B6-D15CD78B0796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53040390-4904-4718-AFF7-B1F0F2571C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -421,6 +421,18 @@
   </si>
   <si>
     <t>Id Funcionário</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>Ítalo</t>
+  </si>
+  <si>
+    <t>italo@mercadofacil.com</t>
+  </si>
+  <si>
+    <t>122001</t>
   </si>
 </sst>
 </file>
@@ -700,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -761,13 +773,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,6 +790,109 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="94">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -965,109 +1080,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2320,29 +2332,29 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H4" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="A1:H4" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2794,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2965,8 +2977,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3168,10 +3181,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540BAB3-B589-4DCB-98FE-D1E262F0FB3A}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,7 +3232,7 @@
       <c r="B2" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="40" t="s">
         <v>109</v>
       </c>
       <c r="D2" s="40" t="s">
@@ -3231,7 +3244,7 @@
       <c r="F2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="43" t="s">
         <v>112</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -3245,7 +3258,7 @@
       <c r="B3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="39" t="s">
         <v>115</v>
       </c>
       <c r="D3" s="39" t="s">
@@ -3257,7 +3270,7 @@
       <c r="F3" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="42" t="s">
         <v>117</v>
       </c>
       <c r="H3" s="39" t="s">
@@ -3271,7 +3284,7 @@
       <c r="B4" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="41" t="s">
         <v>120</v>
       </c>
       <c r="D4" s="41" t="s">
@@ -3283,11 +3296,37 @@
       <c r="F4" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="44" t="s">
         <v>122</v>
       </c>
       <c r="H4" s="41" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3303,7 +3342,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,7 +3381,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,7 +3426,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,7 +3482,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3524,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,7 +3783,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3842,7 +3881,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix: gerenciador e planilha de oferta
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53040390-4904-4718-AFF7-B1F0F2571C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F358BD4-37D5-4BFD-AB14-176181C2C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>122001</t>
+  </si>
+  <si>
+    <t>Qtde Mínima</t>
   </si>
 </sst>
 </file>
@@ -782,14 +785,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="100">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2274,28 +2293,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="99" headerRowBorderDxfId="98" tableBorderDxfId="97" totalsRowBorderDxfId="96">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="95"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2316,45 +2335,45 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="12" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="18" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2408,80 +2427,81 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="74"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="54">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2806,7 +2826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3015,13 +3035,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E75FFB4-713F-4EF0-9034-135108041187}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3322,7 +3345,7 @@
       <c r="F5" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="44" t="s">
         <v>112</v>
       </c>
       <c r="H5" s="41" t="s">
@@ -3780,24 +3803,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E452B3BA-6480-4C31-A0A0-FCD7F2BD6829}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -3808,10 +3832,33 @@
         <v>87</v>
       </c>
       <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="38">
+        <v>5</v>
+      </c>
+      <c r="E2" s="36">
+        <v>45437</v>
+      </c>
+      <c r="F2" s="36">
+        <v>45443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: armazenador de log versão 1
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\Projeto Integrador SEM1 Workspace\mercadoFacil-piSenac-\src\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F358BD4-37D5-4BFD-AB14-176181C2C0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73DE92-9B7B-424A-96B8-46CAF32EC18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -442,7 +442,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +473,14 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -715,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -786,35 +797,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="100">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -824,6 +823,7 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -835,12 +835,11 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
@@ -849,8 +848,6 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -862,15 +859,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -878,6 +866,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -1680,6 +1677,24 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <fill>
@@ -2308,13 +2323,13 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="44" headerRowBorderDxfId="43" tableBorderDxfId="42" totalsRowBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2335,45 +2350,45 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="36" dataDxfId="34" headerRowBorderDxfId="35" tableBorderDxfId="33" totalsRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" insertRow="1" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2463,45 +2478,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="53"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3362,10 +3377,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,7 +3390,7 @@
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>58</v>
       </c>
@@ -3386,10 +3401,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="47">
+        <v>45432.5</v>
+      </c>
+      <c r="C2" s="47">
+        <v>45432.541666666664</v>
+      </c>
+      <c r="G2" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3805,7 +3827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E452B3BA-6480-4C31-A0A0-FCD7F2BD6829}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feature: gerenciador de funcionario
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73DE92-9B7B-424A-96B8-46CAF32EC18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11C5400-0493-4034-974C-1A25CB0F59C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Produto" sheetId="1" r:id="rId1"/>
-    <sheet name="Estoque" sheetId="17" r:id="rId2"/>
+    <sheet name="Estoque" sheetId="17" r:id="rId1"/>
+    <sheet name="Produto" sheetId="1" r:id="rId2"/>
     <sheet name="Vendas" sheetId="15" r:id="rId3"/>
     <sheet name="Venda_Item" sheetId="16" r:id="rId4"/>
     <sheet name="Fornecedores" sheetId="4" r:id="rId5"/>
@@ -24,7 +24,7 @@
     <sheet name="Compra" sheetId="18" r:id="rId9"/>
     <sheet name="Empresa" sheetId="9" r:id="rId10"/>
     <sheet name="Ponto Funcionarios" sheetId="10" r:id="rId11"/>
-    <sheet name="Funcionarios" sheetId="11" r:id="rId12"/>
+    <sheet name="Funcionarios" sheetId="20" r:id="rId12"/>
     <sheet name="Usuarios" sheetId="19" r:id="rId13"/>
     <sheet name="Controle de Acesso" sheetId="14" r:id="rId14"/>
   </sheets>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="131">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Nome</t>
   </si>
   <si>
-    <t>idFuncionario</t>
-  </si>
-  <si>
     <t>CPF</t>
   </si>
   <si>
@@ -436,6 +433,15 @@
   </si>
   <si>
     <t>Qtde Mínima</t>
+  </si>
+  <si>
+    <t>Id Funcionario</t>
+  </si>
+  <si>
+    <t>12345678901</t>
+  </si>
+  <si>
+    <t>enzo@mercadofacil@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -443,9 +449,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,8 +488,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,8 +516,14 @@
         <bgColor rgb="FFFBE2D5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -722,11 +742,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -798,15 +833,26 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="100">
-    <dxf>
-      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+  <dxfs count="88">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -823,7 +869,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="d/m/yy\ h:mm;@"/>
+      <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -859,6 +905,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -866,15 +921,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
@@ -1158,36 +1204,20 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1198,67 +1228,50 @@
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1271,86 +1284,7 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1389,20 +1323,50 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
         <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1410,15 +1374,14 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1426,37 +1389,57 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
         <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1470,6 +1453,9 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1511,47 +1497,51 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
-        <top/>
-        <bottom/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1559,14 +1549,23 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1574,29 +1573,45 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF000000"/>
@@ -1604,27 +1619,95 @@
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1640,7 +1723,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1679,24 +1767,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1731,9 +1801,7 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
+        <right/>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -1779,7 +1847,9 @@
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
         <top style="thin">
           <color rgb="FF000000"/>
         </top>
@@ -1822,33 +1892,7 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
+        <left/>
         <right style="thin">
           <color rgb="FF000000"/>
         </right>
@@ -1952,235 +1996,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <border outline="0">
         <left style="thin">
@@ -2308,28 +2123,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="99" headerRowBorderDxfId="98" tableBorderDxfId="97" totalsRowBorderDxfId="96">
-  <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="92"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="90"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2350,22 +2165,6 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}" name="Tabela10" displayName="Tabela10" ref="A1:G10" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="A1:G10" xr:uid="{4C52B285-52FE-4514-B2F4-047F0F2A36A8}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D0E46053-9ADC-4077-AAC1-A0D04AC10CB7}" name="Nome" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{A0CEB141-E94A-48ED-BD92-5DE4198B132F}" name="idFuncionario" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{BE90B2A0-FC8D-4DD4-B78C-AD4D9582E886}" name="CPF" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{6C6F96C5-B948-4725-B53E-7A57DC7ED986}" name="salario" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{DFAE2761-B975-4F0F-9D6E-EA02A4336155}" name="Cargo Setor" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{4E320E52-58CD-4949-968F-2686EB3707D4}" name="Situação" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{3593D9DD-D8D0-4687-8E49-1C0B9D0A118C}" name="Email" dataDxfId="19"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
@@ -2382,8 +2181,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
@@ -2395,15 +2194,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="87" headerRowBorderDxfId="86" tableBorderDxfId="85" totalsRowBorderDxfId="84">
+  <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="79"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2442,33 +2241,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="89" dataDxfId="87" headerRowBorderDxfId="88" tableBorderDxfId="86" totalsRowBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="81"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="80"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="68"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2478,45 +2277,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="62"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2838,165 +2637,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FCEB4-E501-4D56-BC91-46B2FB941374}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="31">
-        <v>2.9</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="33">
-        <v>7</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="32">
-        <v>2.5</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="33">
-        <v>2</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="34">
-        <v>4</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>13</v>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3051,7 +2729,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,131 +2767,72 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A4EF80-7496-4B05-86B1-54C8E4F6E45F}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D92E029-30E2-4813-B272-76AAF7049503}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>51</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
+      <c r="A2" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="54">
+        <v>1500</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="53" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -3221,8 +2840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540BAB3-B589-4DCB-98FE-D1E262F0FB3A}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3239,132 +2858,132 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>57</v>
-      </c>
       <c r="H1" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="C2" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="D2" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="E2" s="40" t="s">
+      <c r="F2" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="G2" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="43" t="s">
-        <v>112</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="D3" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="39" t="s">
+      <c r="F3" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>117</v>
-      </c>
       <c r="H3" s="39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="C4" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="D4" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" s="41" t="s">
+      <c r="F4" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="44" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>122</v>
-      </c>
       <c r="H4" s="41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="C5" t="s">
         <v>125</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>127</v>
-      </c>
       <c r="F5" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="44" t="s">
-        <v>112</v>
-      </c>
       <c r="H5" s="41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -3379,8 +2998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3392,18 +3011,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="47">
         <v>45432.5</v>
@@ -3422,44 +3041,165 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FCEB4-E501-4D56-BC91-46B2FB941374}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
+    <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="31">
+        <v>2.9</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="33">
+        <v>7</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="32">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="33">
+        <v>2</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="34">
+        <v>4</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3487,31 +3227,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3541,19 +3281,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3585,25 +3325,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>91</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3845,16 +3585,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
       <c r="D1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
@@ -3865,10 +3605,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="45">
         <v>0.1</v>
@@ -3967,10 +3707,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>29</v>
@@ -3996,10 +3736,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="36">
         <v>45402</v>
@@ -4008,7 +3748,7 @@
         <v>2.5</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="37">
         <v>200</v>
@@ -4017,7 +3757,7 @@
         <v>80</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I2" s="36">
         <v>45408</v>

</xml_diff>

<commit_message>
feature: registro de login com log, problema de corrupção Excel
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCBC042-4644-4DF2-9CD6-6B35B207D018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{606D166E-DC80-43A9-AA7D-4050810D9E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="Controle de Acesso" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -761,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -832,8 +833,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,72 +844,89 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="94">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2011,6 +2027,24 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -2147,21 +2181,21 @@
     <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="88"/>
     <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="87"/>
     <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Categoria" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Descrição de produto " dataDxfId="84"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2182,29 +2216,29 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="18" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{72FAEDA4-AA3A-4D1F-9E59-57C1C941D8B7}" name="Email " dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{B44B70BE-4669-4DD0-ACD5-AC883F7D4BF6}" name="Login " dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{DE91924E-F28F-419F-B47A-773261F29055}" name="Senha " dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9FFECF87-F996-4F6F-BEDF-FA3F6A316780}" name="Situação " dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E36D2DC9-D76A-4420-8E03-5EBB7ECD200F}" name="Cargo " dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{6155EBA5-1A2B-410A-B7EB-FE2F8C7EF69C}" name="Id Funcionário" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C2" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:C2" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C4" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2214,12 +2248,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="81"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="79"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2230,14 +2264,14 @@
   <autoFilter ref="A1:I2" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7DA33DF1-70D3-4985-AD72-C7C4CD7A129D}" name="Id Venda"/>
-    <tableColumn id="9" xr3:uid="{26C688A1-DD2C-49A5-9C45-F5670E955BE3}" name="Data"/>
-    <tableColumn id="2" xr3:uid="{B3F389AE-D3A8-4AE7-9533-7F15BEA25591}" name="Hora"/>
-    <tableColumn id="3" xr3:uid="{F3B8F060-BA34-4591-8528-611FE4C95156}" name="Valor Venda"/>
-    <tableColumn id="4" xr3:uid="{F23EAAFB-7C1A-4B89-8679-77D9B852568E}" name="Forma Pagamento"/>
-    <tableColumn id="5" xr3:uid="{BE3D88F9-0263-4A0C-B707-F4991ADEB5D1}" name="Parcelas"/>
-    <tableColumn id="6" xr3:uid="{94D5006F-82D0-4B41-93D5-12F2E5575674}" name="Observações"/>
-    <tableColumn id="7" xr3:uid="{15730F61-DC8B-47AA-A898-94B46456C062}" name="Id Vendedor"/>
-    <tableColumn id="8" xr3:uid="{89AAD5BB-19E7-43F2-9F59-EB4FD699DC56}" name="Id Cliente"/>
+    <tableColumn id="9" xr3:uid="{26C688A1-DD2C-49A5-9C45-F5670E955BE3}" name="Id Cliente"/>
+    <tableColumn id="2" xr3:uid="{B3F389AE-D3A8-4AE7-9533-7F15BEA25591}" name="Data"/>
+    <tableColumn id="3" xr3:uid="{F3B8F060-BA34-4591-8528-611FE4C95156}" name="Hora"/>
+    <tableColumn id="4" xr3:uid="{F23EAAFB-7C1A-4B89-8679-77D9B852568E}" name="Valor Venda"/>
+    <tableColumn id="5" xr3:uid="{BE3D88F9-0263-4A0C-B707-F4991ADEB5D1}" name="Forma Pagamento"/>
+    <tableColumn id="6" xr3:uid="{94D5006F-82D0-4B41-93D5-12F2E5575674}" name="Parcelas"/>
+    <tableColumn id="7" xr3:uid="{15730F61-DC8B-47AA-A898-94B46456C062}" name="Observações"/>
+    <tableColumn id="8" xr3:uid="{89AAD5BB-19E7-43F2-9F59-EB4FD699DC56}" name="Id Vendedor"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2258,33 +2292,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Nome Fornecedor" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Tipo Comércio" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Telefone" dataDxfId="75"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="74"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Documento" dataDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Tipo Comércio" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Nome Fornecedor" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Documento" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="68"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Telefone" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="71" dataDxfId="69" headerRowBorderDxfId="70" tableBorderDxfId="68" totalsRowBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2294,45 +2328,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Desconto" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Qtde Mínima" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Data Inicio" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Fim" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Data Fim" dataDxfId="50"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto" dataDxfId="49"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Qtde Mínima" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Inicio" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="id Produto2" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="Data Solitação" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Valor Unitário" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Unidade Medida" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Valor Total" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Qtde Total" dataDxfId="35"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="id Fornecedor" dataDxfId="34"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="Previsão Entrega" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="Previsão Entrega" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="id Produto2" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Data Solitação" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Valor Unitário" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Unidade Medida" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Valor Total" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="Qtde Total" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2663,12 +2697,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2827,10 +2861,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,11 +2906,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2914,58 +2948,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="47" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="54">
+      <c r="D2" s="52">
         <v>1500</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="51" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2984,14 +3018,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3134,41 +3168,59 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="55" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="56">
         <v>45432.5</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="56">
         <v>45432.541666666664</v>
       </c>
-      <c r="G2" s="48"/>
+      <c r="G2" s="46"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="56">
+        <v>45444.071777245372</v>
+      </c>
+      <c r="C3" s="56"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="57">
+        <v>45444.086656307867</v>
+      </c>
+      <c r="C4" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3182,17 +3234,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74FCEB4-E501-4D56-BC91-46B2FB941374}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3253,13 +3305,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="1" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3309,11 +3361,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3351,13 +3403,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3446,14 +3498,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3602,7 +3654,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E452B3BA-6480-4C31-A0A0-FCD7F2BD6829}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -3610,14 +3662,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,12 +3730,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3732,14 +3784,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feature: gerenciador empresa com verificador, bug ao escrever na planilha
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{606D166E-DC80-43A9-AA7D-4050810D9E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB540CE4-53FA-4772-A17F-E1E7032868EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -443,6 +443,18 @@
   </si>
   <si>
     <t>enzo@mercadofacil@gmail.com</t>
+  </si>
+  <si>
+    <t>Sonda</t>
+  </si>
+  <si>
+    <t>123123</t>
+  </si>
+  <si>
+    <t>Rua 2</t>
+  </si>
+  <si>
+    <t>119999999</t>
   </si>
 </sst>
 </file>
@@ -762,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -774,9 +786,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -859,7 +868,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="94">
+  <dxfs count="95">
     <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1237,7 +1246,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1246,12 +1256,11 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1262,12 +1271,11 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1278,12 +1286,11 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color rgb="FF000000"/>
@@ -1292,8 +1299,6 @@
           <color rgb="FF000000"/>
         </top>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1318,6 +1323,9 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -2174,22 +2182,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="93" headerRowBorderDxfId="92" tableBorderDxfId="91" totalsRowBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92" totalsRowBorderDxfId="91">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="87"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" insertRow="1" totalsRowShown="0" headerRowDxfId="26" headerRowBorderDxfId="25" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
@@ -2233,8 +2241,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C4" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C4" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C8" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
@@ -2248,12 +2256,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2292,33 +2300,33 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" totalsRowBorderDxfId="74">
   <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="72"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Tipo Comércio" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Nome Fornecedor" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Documento" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Telefone" dataDxfId="66"/>
+    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Tipo Comércio" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Nome Fornecedor" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Documento" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Telefone" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="65" dataDxfId="63" headerRowBorderDxfId="64" tableBorderDxfId="62" totalsRowBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2328,45 +2336,45 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Data Fim" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto" dataDxfId="49"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Qtde Mínima" dataDxfId="48"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Inicio" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Data Fim" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Qtde Mínima" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Inicio" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="Previsão Entrega" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="id Produto2" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Data Solitação" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Valor Unitário" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Unidade Medida" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Valor Total" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="Qtde Total" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="Previsão Entrega" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="id Produto2" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Data Solitação" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Valor Unitário" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Unidade Medida" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Valor Total" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="Qtde Total" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2706,16 +2714,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2726,122 +2734,122 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>2.9</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="29">
         <v>2.5</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="30">
         <v>7</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="29">
         <v>2.5</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="28" t="s">
+      <c r="F5" s="25" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="30">
         <v>2</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="31">
         <v>4</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="27" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2857,7 +2865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2C0B43-F228-4CBF-98A3-FF8522669C40}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2868,25 +2878,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2958,48 +2976,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="44" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="52">
+      <c r="D2" s="49">
         <v>1500</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="48" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3029,132 +3047,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="37" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="36" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="38" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="38" t="s">
         <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="38" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3168,10 +3186,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3182,45 +3200,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="52" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="53">
         <v>45432.5</v>
       </c>
-      <c r="C2" s="56">
+      <c r="C2" s="53">
         <v>45432.541666666664</v>
       </c>
-      <c r="G2" s="46"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="56">
+      <c r="B3" s="53">
         <v>45444.071777245372</v>
       </c>
-      <c r="C3" s="56"/>
+      <c r="C3" s="53"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="57">
+      <c r="B4" s="54">
         <v>45444.086656307867</v>
       </c>
-      <c r="C4" s="57"/>
+      <c r="C4" s="54"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="54">
+        <v>45444.091481516203</v>
+      </c>
+      <c r="C5" s="54"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="54">
+        <v>45444.122418749997</v>
+      </c>
+      <c r="C6" s="54"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" s="53">
+        <v>45444.124294965281</v>
+      </c>
+      <c r="C7" s="53"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="54">
+        <v>45444.131129421294</v>
+      </c>
+      <c r="C8" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3268,22 +3322,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="37">
+      <c r="B2" s="34">
         <v>50</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="33">
         <v>45590</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="33">
         <v>45442</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="34">
         <v>82</v>
       </c>
     </row>
@@ -3413,72 +3467,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3509,140 +3563,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3693,22 +3747,22 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="45">
+      <c r="C2" s="42">
         <v>0.1</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="35">
         <v>5</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="33">
         <v>45437</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="33">
         <v>45443</v>
       </c>
     </row>
@@ -3739,32 +3793,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3824,31 +3878,31 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>45402</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="34">
         <v>2.5</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="37">
+      <c r="F2" s="34">
         <v>200</v>
       </c>
-      <c r="G2" s="38">
+      <c r="G2" s="35">
         <v>80</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="36">
+      <c r="I2" s="33">
         <v>45408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: Estrutura Main para Administrador
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB540CE4-53FA-4772-A17F-E1E7032868EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B04B11AC-F1BB-483F-B292-6BE1EC514C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="134">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -445,16 +445,13 @@
     <t>enzo@mercadofacil@gmail.com</t>
   </si>
   <si>
-    <t>Sonda</t>
-  </si>
-  <si>
-    <t>123123</t>
-  </si>
-  <si>
-    <t>Rua 2</t>
-  </si>
-  <si>
-    <t>119999999</t>
+    <t>Adega do Tonhão</t>
+  </si>
+  <si>
+    <t>Rua 3</t>
+  </si>
+  <si>
+    <t>11999999</t>
   </si>
 </sst>
 </file>
@@ -2241,8 +2238,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C8" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C14" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C14" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
@@ -2866,14 +2863,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -2897,13 +2894,13 @@
         <v>131</v>
       </c>
       <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>132</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>133</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3186,10 +3183,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,6 +3272,60 @@
         <v>45444.131129421294</v>
       </c>
       <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="54">
+        <v>45444.632146076387</v>
+      </c>
+      <c r="C9" s="54"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="54">
+        <v>45444.634164814815</v>
+      </c>
+      <c r="C10" s="54"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="53">
+        <v>45444.695902222222</v>
+      </c>
+      <c r="C11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="53">
+        <v>45444.731099039353</v>
+      </c>
+      <c r="C12" s="53"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="53">
+        <v>45444.734502222222</v>
+      </c>
+      <c r="C13" s="53"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="54">
+        <v>45444.740898460645</v>
+      </c>
+      <c r="C14" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feature: gerenciador fornecedores e main para administrador completo
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B04B11AC-F1BB-483F-B292-6BE1EC514C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95AAF2D-596E-4954-B26E-00BC158F2722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
     <sheet name="Estoque" sheetId="17" r:id="rId2"/>
     <sheet name="Vendas" sheetId="15" r:id="rId3"/>
     <sheet name="Venda_Item" sheetId="16" r:id="rId4"/>
-    <sheet name="Fornecedores" sheetId="4" r:id="rId5"/>
+    <sheet name="Fornecedores" sheetId="21" r:id="rId5"/>
     <sheet name="Metas" sheetId="5" r:id="rId6"/>
     <sheet name="Ofertas" sheetId="6" r:id="rId7"/>
     <sheet name="Cliente" sheetId="7" r:id="rId8"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -452,6 +452,24 @@
   </si>
   <si>
     <t>11999999</t>
+  </si>
+  <si>
+    <t>JBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frigorífico </t>
+  </si>
+  <si>
+    <t>1199887411</t>
+  </si>
+  <si>
+    <t>Rua das Carnes</t>
+  </si>
+  <si>
+    <t>Antônio da Fonseca</t>
+  </si>
+  <si>
+    <t>42358768210</t>
   </si>
 </sst>
 </file>
@@ -771,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -861,11 +879,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
+  <dxfs count="83">
     <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1805,235 +1827,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2179,34 +1972,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="94" headerRowBorderDxfId="93" tableBorderDxfId="92" totalsRowBorderDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="86"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="85"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="78"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="77"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="75"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="19"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}" name="Tabela6" displayName="Tabela6" ref="A1:E2" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:E2" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}"/>
   <tableColumns count="5">
@@ -2220,7 +2000,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
   <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
@@ -2237,9 +2017,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C14" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C14" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C17" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C17" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
@@ -2253,12 +2033,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="83"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="82"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="81"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="80"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="79"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2297,22 +2077,6 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}" name="Tabela3" displayName="Tabela3" ref="A1:G6" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" totalsRowBorderDxfId="74">
-  <autoFilter ref="A1:G6" xr:uid="{FE028123-DCE2-4C67-91CC-9DB9E7DEAB00}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1E1F1B9F-C2EC-481E-A5BA-E32211033C0D}" name="Id Fornecedor" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{5B7AE8DB-5B49-4D37-B548-ACC50F17A08E}" name="Tipo Comércio" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{F38AB42E-31F7-4399-8A30-8F6DA322186C}" name="Nome Fornecedor" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{9FAD8597-53B1-4C0B-8104-4E4FC70C977E}" name="Documento" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{9210E803-4788-4DBB-985A-19EEC6D3D962}" name="Endereço" dataDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{73579FA2-8EBD-476F-A461-7179AA3AE59B}" name="Responsável" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{23291954-A70D-4B20-B88D-0DAAEAB17747}" name="Telefone" dataDxfId="67"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
   <tableColumns count="8">
@@ -2329,7 +2093,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
   <tableColumns count="6">
@@ -2344,7 +2108,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44">
   <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
@@ -2359,7 +2123,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="37">
   <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
   <tableColumns count="9">
@@ -2374,6 +2138,19 @@
     <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
+  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3183,7 +2960,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -3326,6 +3103,33 @@
         <v>45444.740898460645</v>
       </c>
       <c r="C14" s="54"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="54">
+        <v>45444.788243807867</v>
+      </c>
+      <c r="C15" s="54"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="53">
+        <v>45444.802933344909</v>
+      </c>
+      <c r="C16" s="53"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="54">
+        <v>45444.803800486108</v>
+      </c>
+      <c r="C17" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3499,97 +3303,72 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B46210-C88C-4D3D-AA28-7F5B038AF542}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF04CEFE-ECC5-4A02-8182-CE6018512D80}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="44" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
+      <c r="A2" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feature: preenchendo dados de funcionarios no excel
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E95AAF2D-596E-4954-B26E-00BC158F2722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3018ED14-CD63-4578-AE72-7344F316CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Vendas" sheetId="15" r:id="rId3"/>
     <sheet name="Venda_Item" sheetId="16" r:id="rId4"/>
     <sheet name="Fornecedores" sheetId="21" r:id="rId5"/>
-    <sheet name="Metas" sheetId="5" r:id="rId6"/>
+    <sheet name="Metas" sheetId="22" r:id="rId6"/>
     <sheet name="Ofertas" sheetId="6" r:id="rId7"/>
     <sheet name="Cliente" sheetId="7" r:id="rId8"/>
     <sheet name="Compra" sheetId="18" r:id="rId9"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="147">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Bonificação</t>
   </si>
   <si>
-    <t>idVendedor</t>
-  </si>
-  <si>
     <t>idCaixa</t>
   </si>
   <si>
@@ -442,9 +439,6 @@
     <t>12345678901</t>
   </si>
   <si>
-    <t>enzo@mercadofacil@gmail.com</t>
-  </si>
-  <si>
     <t>Adega do Tonhão</t>
   </si>
   <si>
@@ -470,6 +464,33 @@
   </si>
   <si>
     <t>42358768210</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>01123456789</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>Alonso</t>
+  </si>
+  <si>
+    <t>00112233445</t>
+  </si>
+  <si>
+    <t>alonso@mercadofacil.com</t>
+  </si>
+  <si>
+    <t>987654</t>
+  </si>
+  <si>
+    <t>11223344556</t>
+  </si>
+  <si>
+    <t>22334455667</t>
   </si>
 </sst>
 </file>
@@ -496,13 +517,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -524,8 +538,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,8 +571,14 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -601,19 +628,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -654,28 +668,6 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -751,19 +743,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -789,7 +768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -800,94 +779,578 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="81">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1017,195 +1480,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color rgb="FF000000"/>
@@ -1572,261 +1846,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF000000"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1972,37 +1991,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="82" headerRowBorderDxfId="81" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78" totalsRowBorderDxfId="77">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="75"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}" name="Tabela6" displayName="Tabela6" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D05168A4-7494-42E3-80CA-A5EF91D04256}" name="data"/>
-    <tableColumn id="2" xr3:uid="{9125E824-2504-4B0E-957D-030859DB5451}" name="id Funcionario"/>
-    <tableColumn id="3" xr3:uid="{A0BF47A2-E842-4FA4-A386-D0024C55EB45}" name="Horario Saída"/>
-    <tableColumn id="4" xr3:uid="{FB70219B-2083-4B01-9D13-7727ECC20C12}" name="Horario Entrada"/>
-    <tableColumn id="5" xr3:uid="{FEE7D022-5791-4930-BF05-5D2D5A1660B7}" name="Tempo Atraso"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F7C378A-CDD2-4CA8-A3A2-DFD898446D04}" name="Tabela1" displayName="Tabela1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowBorderDxfId="17" tableBorderDxfId="18">
+  <autoFilter ref="A1:G6" xr:uid="{2F7C378A-CDD2-4CA8-A3A2-DFD898446D04}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{B9986DEC-FE67-440F-A0C3-9F948A677BBC}" name="Id Funcionario" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CE445E75-B683-48E7-8DFE-882ACE9641CE}" name="Nome" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{250DD343-B531-47B6-9E3F-82B07D4FF142}" name="CPF" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{A20D1E40-5883-463C-8752-347FF693D8B5}" name="salario" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FACF4060-77D4-417E-985B-C90F45ACE109}" name="Cargo Setor" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{8119759B-B7DD-4F24-9052-47FE3C5CC391}" name="Situação" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A31856D8-75A1-4BA7-84C8-432982ECF510}" name="Email" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="A1:H5" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}" name="Tabela7" displayName="Tabela7" ref="A1:H6" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A1:H6" xr:uid="{597E9F5B-61B8-4C91-9E9B-39967C9DDBCB}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B7D99FB7-686E-4691-9670-BB762F92C6B8}" name="ID Usuario" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{56D552BF-5E52-4346-8232-19E7545A7861}" name="Nome " dataDxfId="13"/>
@@ -2018,12 +2039,12 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C17" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C17" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A1:C17" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{08CBA582-0320-4BD5-94F6-FD3F883700A1}" name="Horario Logoff" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2033,12 +2054,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="67"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2077,78 +2098,75 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}" name="Tabela9" displayName="Tabela9" ref="A1:H12" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
-  <autoFilter ref="A1:H12" xr:uid="{9E40C1AB-3743-4A45-A9B3-E7FCAB29F10D}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B0779E67-9AD9-4DD8-895B-E180CE360579}" name="id Meta" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{847FC979-558E-4ADC-93DC-8DD3840F1E0D}" name="Valor Da Meta" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{4AFF2D48-6EEC-46AF-83A9-6229E1FDCC5E}" name="Bonificação" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{4A265D49-5D41-49B3-9042-08A51ED464AE}" name="idVendedor" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{78083FE3-2564-4017-B7DE-9E1B2A968873}" name="idCaixa" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{D83AE102-34B6-4132-9DE2-519F7EDDB449}" name="Data Inicio" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{B0322598-C985-448E-9F8C-7BB458A37076}" name="Data Final" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{C004F583-440F-45BF-9F57-3837B3400DA9}" name="Valor de Vendas" dataDxfId="54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
+  <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Data Fim" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Qtde Mínima" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Inicio" dataDxfId="59"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}" name="Tabela2" displayName="Tabela2" ref="A1:F2" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{244BD417-3AA6-4E4B-A404-585DD08BD408}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="58" dataDxfId="56" headerRowBorderDxfId="57" tableBorderDxfId="55">
+  <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{52F86E01-31E1-4016-8E39-1F4EA750C7DE}" name="Id Oferta" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{769CF79D-428F-43AF-8A36-49C68593221A}" name="Id Produto" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{CE468A4B-F255-4DA3-9DF6-C91418FA3F0B}" name="Data Fim" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{4B13455F-08ED-4805-B42B-F6FAC3D65426}" name="Desconto" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{59E45DA3-22E3-4138-82FB-38A8BE23981F}" name="Qtde Mínima" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{D7C8A978-FA4C-4949-B0F9-083CCAA6643D}" name="Data Inicio" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}" name="Tabela4" displayName="Tabela4" ref="A1:F2" insertRow="1" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44">
-  <autoFilter ref="A1:F2" xr:uid="{019082B4-1BD9-4BF9-ACA3-3E40D0E08E16}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7F58A073-4EFD-4873-8A51-7DC9DBC449A3}" name="Nome " dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{E1A8F338-21F9-4115-9688-8F68214663F9}" name="CPF " dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{841CB8C9-4F64-4B62-AA95-82194C4BC978}" name="CEP " dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{1C23CE5F-8EF9-41ED-9F45-5982157C7D2C}" name="Data Nascimento " dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{8AF4247F-77A5-4F96-8857-78B04E028144}" name="Telefone " dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{EA9D1A60-8DE7-4D03-8DF5-C9C167D308D6}" name="ID Cliente" dataDxfId="38"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="48">
+  <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="Previsão Entrega" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="id Produto2" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Data Solitação" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Valor Unitário" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Unidade Medida" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Valor Total" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="Qtde Total" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}" name="Tabela19" displayName="Tabela19" ref="A1:I2" totalsRowShown="0" headerRowDxfId="37">
-  <autoFilter ref="A1:I2" xr:uid="{F0278D3D-182E-4CB5-B5BB-7213B093E75D}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A6C36C0E-1EED-4A3C-A303-957C48677B98}" name="id Compra" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{3B02A782-19EC-4F71-B521-7C8EFF54D18E}" name="Previsão Entrega" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{90F59BE5-FFBA-4351-B11F-F2FB1E89CD06}" name="id Produto2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{3BDA4226-6506-4916-BEF2-6C9EB1690999}" name="Data Solitação" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00D1DD03-5A1E-4194-80B6-E25A2E557F78}" name="Valor Unitário" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{4C4251A0-4F4F-461B-BD00-38300E4002F5}" name="Unidade Medida" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{3B263ECD-AA90-4A5D-ADCA-FB4176B2E171}" name="Valor Total" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{9FECB700-6C19-42E1-9BD1-80ED7869999B}" name="Qtde Total" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{E0D3F4E8-B6A8-444F-A9D3-F0D554B8FE53}" name="id Fornecedor" dataDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}" name="Tabela5" displayName="Tabela5" ref="A1:D2" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
-  <autoFilter ref="A1:D2" xr:uid="{D2655A56-3B61-4DB3-9815-400EF79DBC6D}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{83D0C318-5E99-4CA6-9926-892DFFA553E8}" name="Razao Social " dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{74E54BE1-CE70-4F66-B328-23BF8CF42A43}" name="CNPJ" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{B90E473A-BD07-4C1A-9D4B-F76A68A34F2F}" name="Endereço " dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{E07AB348-F6CE-42A3-B494-3BD2C376761E}" name="Telefone" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}" name="Tabela6" displayName="Tabela6" ref="A1:E2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:E2" xr:uid="{6EE29E44-FD64-48FD-B85A-E648DFD03C71}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D05168A4-7494-42E3-80CA-A5EF91D04256}" name="data"/>
+    <tableColumn id="2" xr3:uid="{9125E824-2504-4B0E-957D-030859DB5451}" name="id Funcionario"/>
+    <tableColumn id="3" xr3:uid="{A0BF47A2-E842-4FA4-A386-D0024C55EB45}" name="Horario Saída"/>
+    <tableColumn id="4" xr3:uid="{FB70219B-2083-4B01-9D13-7727ECC20C12}" name="Horario Entrada"/>
+    <tableColumn id="5" xr3:uid="{FEE7D022-5791-4930-BF05-5D2D5A1660B7}" name="Tempo Atraso"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2488,142 +2506,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="17">
+        <v>2.9</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="19">
+        <v>7</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="20">
         <v>4</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="28">
-        <v>2.9</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="E7" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="29">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="30">
-        <v>7</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="29">
-        <v>2.5</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="30">
-        <v>2</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="31">
-        <v>4</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2653,31 +2671,31 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
         <v>131</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D2" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2707,19 +2725,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2732,80 +2750,175 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D92E029-30E2-4813-B272-76AAF7049503}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="51">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="50" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="46" t="s">
+      <c r="D3" s="51">
+        <v>1500</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="49">
-        <v>1500</v>
-      </c>
-      <c r="E2" s="47" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="B4" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="51">
+        <v>2500</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="54" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="51">
+        <v>2000</v>
+      </c>
+      <c r="E5" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="48" t="s">
-        <v>130</v>
+      <c r="F5" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" s="51">
+        <v>1400</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0540BAB3-B589-4DCB-98FE-D1E262F0FB3A}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,133 +2934,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="37" t="s">
+      <c r="B5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="G5" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="36" t="s">
+      <c r="H5" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="F3" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>123</v>
+      <c r="H6" s="25" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2962,7 +3101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2974,162 +3113,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="52" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="53">
+      <c r="A2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="38">
         <v>45432.5</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="38">
         <v>45432.541666666664</v>
       </c>
-      <c r="G2" s="43"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="53">
+      <c r="A3" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="38">
         <v>45444.071777245372</v>
       </c>
-      <c r="C3" s="53"/>
+      <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="54">
+      <c r="A4" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="39">
         <v>45444.086656307867</v>
       </c>
-      <c r="C4" s="54"/>
+      <c r="C4" s="39"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="54">
+      <c r="A5" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="39">
         <v>45444.091481516203</v>
       </c>
-      <c r="C5" s="54"/>
+      <c r="C5" s="39"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B6" s="54">
+      <c r="A6" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="39">
         <v>45444.122418749997</v>
       </c>
-      <c r="C6" s="54"/>
+      <c r="C6" s="39"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7" s="53">
+      <c r="A7" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="38">
         <v>45444.124294965281</v>
       </c>
-      <c r="C7" s="53"/>
+      <c r="C7" s="38"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="54">
+      <c r="A8" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="39">
         <v>45444.131129421294</v>
       </c>
-      <c r="C8" s="54"/>
+      <c r="C8" s="39"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="54">
+      <c r="A9" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="39">
         <v>45444.632146076387</v>
       </c>
-      <c r="C9" s="54"/>
+      <c r="C9" s="39"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="54">
+      <c r="A10" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="39">
         <v>45444.634164814815</v>
       </c>
-      <c r="C10" s="54"/>
+      <c r="C10" s="39"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" s="53">
+      <c r="A11" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="38">
         <v>45444.695902222222</v>
       </c>
-      <c r="C11" s="53"/>
+      <c r="C11" s="38"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12" s="53">
+      <c r="A12" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="38">
         <v>45444.731099039353</v>
       </c>
-      <c r="C12" s="53"/>
+      <c r="C12" s="38"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="53">
+      <c r="A13" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="38">
         <v>45444.734502222222</v>
       </c>
-      <c r="C13" s="53"/>
+      <c r="C13" s="38"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B14" s="54">
+      <c r="A14" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="39">
         <v>45444.740898460645</v>
       </c>
-      <c r="C14" s="54"/>
+      <c r="C14" s="39"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="54">
+      <c r="A15" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="39">
         <v>45444.788243807867</v>
       </c>
-      <c r="C15" s="54"/>
+      <c r="C15" s="39"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B16" s="53">
+      <c r="A16" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="38">
         <v>45444.802933344909</v>
       </c>
-      <c r="C16" s="53"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="54">
+      <c r="A17" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="39">
         <v>45444.803800486108</v>
       </c>
-      <c r="C17" s="54"/>
+      <c r="C17" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3158,41 +3297,41 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="34">
+      <c r="A2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="23">
         <v>50</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="33">
+      <c r="C2" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="22">
         <v>45590</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="22">
         <v>45442</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="23">
         <v>82</v>
       </c>
     </row>
@@ -3225,31 +3364,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>67</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" t="s">
         <v>72</v>
-      </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3279,19 +3418,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3322,49 +3461,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="D1" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="F1" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="56" t="s">
+      <c r="A2" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="E2" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="F2" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="G2" s="34" t="s">
         <v>137</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="G2" s="48" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3373,166 +3512,79 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490B7451-1A7F-4FCB-BE82-E7B49B8D5224}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F389CF-B47B-4D13-8A68-5CB39260CAE0}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
+      <c r="A2" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="44">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="44">
+        <v>100</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="45">
+        <v>45413</v>
+      </c>
+      <c r="G2" s="45">
+        <v>45443</v>
+      </c>
+      <c r="H2" s="46">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -3558,41 +3610,41 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="42">
+      <c r="A2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="28">
         <v>0.1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="24">
         <v>5</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="22">
         <v>45437</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="22">
         <v>45443</v>
       </c>
     </row>
@@ -3624,22 +3676,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3680,59 +3732,59 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="A2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="22">
         <v>45402</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="23">
         <v>2.5</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="34">
+      <c r="E2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="23">
         <v>200</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2" s="24">
         <v>80</v>
       </c>
-      <c r="H2" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="I2" s="33">
+      <c r="H2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="22">
         <v>45408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: main com Metas
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
@@ -31,7 +31,7 @@
   <calcPr calcId="191028"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="148">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -2838,12 +2838,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3004,10 +3004,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3057,11 +3057,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3099,13 +3099,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3264,14 +3264,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3448,9 +3448,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3610,6 +3610,14 @@
         <v>45444.803800486108</v>
       </c>
       <c r="C17" s="39"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" t="n">
+        <v>45444.8614434375</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3629,11 +3637,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3694,13 +3702,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3750,11 +3758,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3792,13 +3800,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3862,14 +3870,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3968,14 +3976,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4036,12 +4044,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -4090,14 +4098,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feature: Main para caixa e Gerente com Gerenciador de Venda e correção para impressão de data e horários
</commit_message>
<xml_diff>
--- a/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
+++ b/src/resource/ExcelAsADatabaseMercadoFacil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo Afonso\Desktop\Nova pasta\mercadoFacil-piSenac-\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{F109E781-C1BF-4B69-9829-16E49D4240E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB3A90B6-425C-44A8-BC62-3FE34393F3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produto" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="158">
   <si>
     <t>Id do Produto</t>
   </si>
@@ -512,14 +512,27 @@
   </si>
   <si>
     <t>11999999999</t>
+  </si>
+  <si>
+    <t>000001</t>
+  </si>
+  <si>
+    <t>Débito</t>
+  </si>
+  <si>
+    <t>000000001</t>
+  </si>
+  <si>
+    <t>000000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -789,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,14 +892,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
+  <dxfs count="105">
     <dxf>
       <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -2188,6 +2199,45 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -2330,15 +2380,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="91" headerRowBorderDxfId="90" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}" name="Tabela12" displayName="Tabela12" ref="A1:F7" totalsRowShown="0" headerRowDxfId="104" headerRowBorderDxfId="103" tableBorderDxfId="102" totalsRowBorderDxfId="101">
   <autoFilter ref="A1:F7" xr:uid="{D879337A-24D0-4711-82E6-5C71994E4D19}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="86"/>
-    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="85"/>
-    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{8A020CFD-C331-44DC-891D-30B04ED42153}" name="Id do Produto" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{F14FB813-4895-4F70-A855-B5636829BF22}" name="Nome do Produto" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{60153C83-78D1-44E5-824A-FFF35C26D71F}" name="Código de Barra" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{47BEDAAE-32EF-4991-8790-4AC543F52E63}" name="Valor do Produto " dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{2F4A7EE6-C6CA-4DCE-BFD5-4F9DC42BA445}" name="Descrição de produto " dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{60568A12-27C7-40A1-A3EC-40E6E508EF15}" name="Categoria" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2392,8 +2442,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C23" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C23" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}" name="Tabela11" displayName="Tabela11" ref="A1:C38" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:C38" xr:uid="{8D3879D7-3E7E-4A1E-9052-8B640565EAD7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{99B352CC-4032-484A-A289-3563233D6D5E}" name="ID Usuario " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00AEE870-6581-46A3-AE80-E9DCFEC12F19}" name="Horario Login" dataDxfId="1"/>
@@ -2407,43 +2457,43 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}" name="Tabela15" displayName="Tabela15" ref="A1:F2" totalsRowShown="0">
   <autoFilter ref="A1:F2" xr:uid="{3797A3FB-BFF2-4143-9325-A8C23A7D7BB5}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{C9F8D13A-A0CD-463F-8D44-B90C09FF19B2}" name="Id Produto" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{6B31F83A-F594-40EE-8A42-AD002F9CE874}" name="Quantidade" dataDxfId="93"/>
+    <tableColumn id="3" xr3:uid="{DB81377F-C06F-41FA-97F0-E3DDADF088CA}" name="Id Lote" dataDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{5EAF71CB-35D5-4028-B280-B9710429BBD3}" name="Data Validade" dataDxfId="91"/>
+    <tableColumn id="5" xr3:uid="{09E5EDF1-B61E-4E57-AFB3-EA60CF2B94A7}" name="Data Entrada" dataDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{72B63C26-9FE5-4DBB-8798-52369138E324}" name="Custo" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}" name="Tabela13" displayName="Tabela13" ref="A1:I2" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}" name="Tabela13" displayName="Tabela13" ref="A1:I2" totalsRowShown="0">
   <autoFilter ref="A1:I2" xr:uid="{B8CAB12E-65F4-4E76-8903-E13139612F6E}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{7DA33DF1-70D3-4985-AD72-C7C4CD7A129D}" name="Id Venda"/>
-    <tableColumn id="9" xr3:uid="{26C688A1-DD2C-49A5-9C45-F5670E955BE3}" name="Id Cliente"/>
-    <tableColumn id="2" xr3:uid="{B3F389AE-D3A8-4AE7-9533-7F15BEA25591}" name="Data"/>
-    <tableColumn id="3" xr3:uid="{F3B8F060-BA34-4591-8528-611FE4C95156}" name="Hora"/>
-    <tableColumn id="4" xr3:uid="{F23EAAFB-7C1A-4B89-8679-77D9B852568E}" name="Valor Venda"/>
-    <tableColumn id="5" xr3:uid="{BE3D88F9-0263-4A0C-B707-F4991ADEB5D1}" name="Forma Pagamento"/>
-    <tableColumn id="6" xr3:uid="{94D5006F-82D0-4B41-93D5-12F2E5575674}" name="Parcelas"/>
-    <tableColumn id="7" xr3:uid="{15730F61-DC8B-47AA-A898-94B46456C062}" name="Observações"/>
-    <tableColumn id="8" xr3:uid="{89AAD5BB-19E7-43F2-9F59-EB4FD699DC56}" name="Id Vendedor"/>
+    <tableColumn id="1" xr3:uid="{7DA33DF1-70D3-4985-AD72-C7C4CD7A129D}" name="Id Venda" dataDxfId="88"/>
+    <tableColumn id="9" xr3:uid="{26C688A1-DD2C-49A5-9C45-F5670E955BE3}" name="Id Cliente" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{B3F389AE-D3A8-4AE7-9533-7F15BEA25591}" name="Data" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{F3B8F060-BA34-4591-8528-611FE4C95156}" name="Hora" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{F23EAAFB-7C1A-4B89-8679-77D9B852568E}" name="Valor Venda" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{BE3D88F9-0263-4A0C-B707-F4991ADEB5D1}" name="Forma Pagamento" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{94D5006F-82D0-4B41-93D5-12F2E5575674}" name="Parcelas" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{15730F61-DC8B-47AA-A898-94B46456C062}" name="Observações" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{89AAD5BB-19E7-43F2-9F59-EB4FD699DC56}" name="Id Vendedor" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}" name="Tabela14" displayName="Tabela14" ref="A1:E2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}" name="Tabela14" displayName="Tabela14" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3" xr:uid="{C5B9F53E-85A8-41F0-966E-5EF9AF840109}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6A285388-05C3-4250-931A-479D682F6087}" name="Id Item Venda"/>
-    <tableColumn id="2" xr3:uid="{13A3B266-03F3-4868-A4D9-FC39B364494E}" name="Venda Id"/>
-    <tableColumn id="3" xr3:uid="{C6DD3B99-EBEF-4F4B-96E3-96DC3228A5FD}" name="Produto Id"/>
-    <tableColumn id="4" xr3:uid="{685D0BE6-1F42-4049-BE66-811D246CDE37}" name="Quantidade"/>
+    <tableColumn id="1" xr3:uid="{6A285388-05C3-4250-931A-479D682F6087}" name="Id Item Venda" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{13A3B266-03F3-4868-A4D9-FC39B364494E}" name="Venda Id" dataDxfId="78"/>
+    <tableColumn id="3" xr3:uid="{C6DD3B99-EBEF-4F4B-96E3-96DC3228A5FD}" name="Produto Id" dataDxfId="77"/>
+    <tableColumn id="4" xr3:uid="{685D0BE6-1F42-4049-BE66-811D246CDE37}" name="Quantidade" dataDxfId="76"/>
     <tableColumn id="5" xr3:uid="{20C600D2-E04C-46CF-B028-B45422F121D1}" name="Valor Item"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3455,9 +3505,9 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E33E2C1-30A3-454F-977B-25D7432E81BC}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3679,6 +3729,141 @@
         <v>45444.910084710646</v>
       </c>
       <c r="C23" s="36"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="35">
+        <v>45444.974817754628</v>
+      </c>
+      <c r="C24" s="35"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="35">
+        <v>45444.977456562498</v>
+      </c>
+      <c r="C25" s="35"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="36">
+        <v>45444.979467488425</v>
+      </c>
+      <c r="C26" s="36"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="35">
+        <v>45444.981828819444</v>
+      </c>
+      <c r="C27" s="35"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="35">
+        <v>45444.982755104167</v>
+      </c>
+      <c r="C28" s="35"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" s="35">
+        <v>45444.983143020836</v>
+      </c>
+      <c r="C29" s="35"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="35">
+        <v>45444.984243240739</v>
+      </c>
+      <c r="C30" s="35"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="35">
+        <v>45444.985149780092</v>
+      </c>
+      <c r="C31" s="35"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="35">
+        <v>45444.986284895836</v>
+      </c>
+      <c r="C32" s="35"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="35">
+        <v>45444.989803356482</v>
+      </c>
+      <c r="C33" s="35"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="35">
+        <v>45444.992578275465</v>
+      </c>
+      <c r="C34" s="35"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="35">
+        <v>45444.99363128472</v>
+      </c>
+      <c r="C35" s="35"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="36">
+        <v>45444.996710810185</v>
+      </c>
+      <c r="C36" s="36"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="36">
+        <v>45444.999516689815</v>
+      </c>
+      <c r="C37" s="36"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="36">
+        <v>45445.034772604165</v>
+      </c>
+      <c r="C38" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3755,10 +3940,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874DB2D-2BBA-4881-96E3-9EC756E4450A}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3801,6 +3986,33 @@
         <v>67</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="19">
+        <v>45442</v>
+      </c>
+      <c r="C2" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="20">
+        <v>100</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" s="21">
+        <v>0</v>
+      </c>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
@@ -3811,10 +4023,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124AE1B6-FA2F-480E-B92D-4A36EA8A4444}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3841,6 +4053,40 @@
       </c>
       <c r="E1" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="20">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="20">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4032,7 +4278,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4099,7 +4345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13400A9C-35AF-4D1A-A093-BF6B7D89743A}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4154,22 +4400,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="51" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="52">
         <v>36739</v>
       </c>
     </row>

</xml_diff>